<commit_message>
Commit perubahan untuk term condition di cek list semua pada saat NAP saja biar gampang pada saat PO dan go live
</commit_message>
<xml_diff>
--- a/Data testing Excel/Parameter New Bike.xlsx
+++ b/Data testing Excel/Parameter New Bike.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="110" windowWidth="14810" windowHeight="8010" tabRatio="864" activeTab="3"/>
+    <workbookView xWindow="240" yWindow="110" windowWidth="14810" windowHeight="8010" tabRatio="864" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Product" sheetId="6" r:id="rId1"/>
@@ -586,7 +586,7 @@
   <numFmts count="1">
     <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -985,14 +985,14 @@
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="7.54296875" customWidth="1"/>
     <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="65.6328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>7</v>
       </c>
@@ -1003,7 +1003,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -1014,7 +1014,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>12</v>
       </c>
@@ -1039,11 +1039,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="7.54296875" customWidth="1"/>
     <col min="2" max="2" width="13.7265625" bestFit="1" customWidth="1"/>
@@ -1052,7 +1052,7 @@
     <col min="5" max="5" width="8.08984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>7</v>
       </c>
@@ -1069,9 +1069,9 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B2" t="s">
         <v>1</v>
@@ -1086,9 +1086,9 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B3" t="s">
         <v>8</v>
@@ -1124,7 +1124,7 @@
       <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="7.54296875" customWidth="1"/>
     <col min="2" max="2" width="5.7265625" bestFit="1" customWidth="1"/>
@@ -1142,7 +1142,7 @@
     <col min="15" max="15" width="9.6328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>7</v>
       </c>
@@ -1189,7 +1189,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:15">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -1236,7 +1236,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="3" spans="1:15">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -1283,7 +1283,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="4" spans="1:15">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>12</v>
       </c>
@@ -1330,7 +1330,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="5" spans="1:15">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>11</v>
       </c>
@@ -1433,11 +1433,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="10.81640625" customWidth="1"/>
     <col min="2" max="2" width="24.26953125" bestFit="1" customWidth="1"/>
@@ -1461,7 +1461,7 @@
     <col min="20" max="20" width="10.08984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>7</v>
       </c>
@@ -1523,7 +1523,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="2" spans="1:20">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -1585,7 +1585,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="3" spans="1:20">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>12</v>
       </c>
@@ -1679,9 +1679,9 @@
       <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:15">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>7</v>
       </c>
@@ -1728,7 +1728,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="2" spans="1:15">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -1761,7 +1761,7 @@
       <c r="N2" s="2"/>
       <c r="O2" s="2"/>
     </row>
-    <row r="3" spans="1:15">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -1796,7 +1796,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="4" spans="1:15">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>11</v>
       </c>
@@ -1843,7 +1843,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="5" spans="1:15">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>11</v>
       </c>
@@ -1900,9 +1900,9 @@
       <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>7</v>
       </c>
@@ -1931,7 +1931,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -1958,7 +1958,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -1987,7 +1987,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>11</v>
       </c>
@@ -2006,7 +2006,7 @@
       <c r="H4" s="2"/>
       <c r="I4" s="2"/>
     </row>
-    <row r="5" spans="1:9">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>12</v>
       </c>
@@ -2031,7 +2031,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="6" spans="1:9">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -2087,7 +2087,7 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="3.90625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.1796875" bestFit="1" customWidth="1"/>
@@ -2107,7 +2107,7 @@
     <col min="17" max="17" width="17.36328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>7</v>
       </c>
@@ -2163,7 +2163,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="2" spans="1:18">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -2217,7 +2217,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:18">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -2271,17 +2271,17 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:18">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:18">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:18">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -2314,7 +2314,7 @@
       <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="16.6328125" customWidth="1"/>
     <col min="2" max="2" width="16.36328125" bestFit="1" customWidth="1"/>
@@ -2325,7 +2325,7 @@
     <col min="7" max="7" width="25.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>7</v>
       </c>
@@ -2348,7 +2348,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -2371,7 +2371,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -2394,7 +2394,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>11</v>
       </c>
@@ -2417,7 +2417,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>11</v>
       </c>
@@ -2432,7 +2432,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="C6" s="15"/>
       <c r="D6" s="15"/>
       <c r="E6" s="15"/>
@@ -2457,7 +2457,7 @@
       <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="3.90625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="7.6328125" bestFit="1" customWidth="1"/>
@@ -2470,7 +2470,7 @@
     <col min="9" max="9" width="24.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>7</v>
       </c>
@@ -2499,7 +2499,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -2525,7 +2525,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>12</v>
       </c>
@@ -2551,12 +2551,12 @@
         <v>178</v>
       </c>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:9">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>11</v>
       </c>

</xml_diff>